<commit_message>
Product search test cases started
</commit_message>
<xml_diff>
--- a/TestData/AutomationExercise/Excel_TestData.xlsx
+++ b/TestData/AutomationExercise/Excel_TestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunvalentine/Documents/Computer Programming/Projects/PlaywrightAutomation/TestData/AutomationExercise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D7F985-027D-FF43-BC2C-5056BACCBBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF75AA3A-BB38-D14F-9E0F-283D8F791E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26640" xr2:uid="{F16CC3AB-E00E-8C4E-8AB8-FF5D31DC8D28}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26640" activeTab="1" xr2:uid="{F16CC3AB-E00E-8C4E-8AB8-FF5D31DC8D28}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Search" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -63,6 +65,39 @@
   </si>
   <si>
     <t>Mamba24!</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>subcategory</t>
+  </si>
+  <si>
+    <t>WOMEN</t>
+  </si>
+  <si>
+    <t>DRESS</t>
+  </si>
+  <si>
+    <t>TOPS</t>
+  </si>
+  <si>
+    <t>SAREE</t>
+  </si>
+  <si>
+    <t>MEN</t>
+  </si>
+  <si>
+    <t>TSHIRTS</t>
+  </si>
+  <si>
+    <t>JEANS</t>
+  </si>
+  <si>
+    <t>KIDS</t>
+  </si>
+  <si>
+    <t>TOPS &amp; SHIRTS</t>
   </si>
 </sst>
 </file>
@@ -447,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF75FD-AAD4-884E-A798-DDCE86BE64BE}">
   <dimension ref="A4:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,4 +532,100 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7B4B67-FB9D-984E-A173-8EC77BD219F5}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37487711-E182-6145-9F6D-976779C6BA80}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>